<commit_message>
Azure and Second Part
</commit_message>
<xml_diff>
--- a/BookStoreAdminApplication/BookStoreAdminApplication/files/users.xlsx
+++ b/BookStoreAdminApplication/BookStoreAdminApplication/files/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop\Desktop\IS-project\BookStore\BookStoreAdminApplication\BookStoreAdminApplication\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4082B4-3134-4C0D-98E8-151221039C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A182A87F-6AFC-445A-9CF3-4E1040565B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4176" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>test3@test.com</t>
   </si>
   <si>
-    <t>test4@test.com</t>
+    <t>t@t.com</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>